<commit_message>
add working hours for story 2
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
+++ b/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umutaktas/Documents/GitHub/real_estate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4E8F0F-63F8-E544-B4E9-E9E7F1F1FACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F43D005-3C31-8A4A-8E64-C7E11136DD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1060" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4220" yWindow="1020" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Subject</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>Completed the implementation of the splash screen and launcher icon</t>
+  </si>
+  <si>
+    <t>20-21.07.2024</t>
+  </si>
+  <si>
+    <t>User story 2 completed</t>
+  </si>
+  <si>
+    <t>Completed location, search, house feed, ordering houses</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1721,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1794,10 +1803,18 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="15"/>
+      <c r="A6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="17">
+        <v>12</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
@@ -1991,7 +2008,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>4.5</v>
+        <v>16.5</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
update user story 3 complete
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
+++ b/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umutaktas/Documents/GitHub/real_estate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B232A134-F669-2247-ADBC-96408DC1FF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813748D4-16BD-E748-9696-83C55CF53BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4220" yWindow="1020" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +24,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -94,7 +96,7 @@
     <t>User story 2 completed</t>
   </si>
   <si>
-    <t>Completed location, search, house feed, ordering houses. House fetching  and business logic unit tests</t>
+    <t>Completed location, search, house feed, ordering houses, animations for detail screen and localization. House fetching  and business logic unit tests</t>
   </si>
 </sst>
 </file>
@@ -449,6 +451,9 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -460,9 +465,6 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1724,7 +1726,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1738,22 +1740,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
@@ -1815,7 +1817,7 @@
       <c r="C6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="20"/>

</xml_diff>

<commit_message>
update record for user story 4
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
+++ b/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umutaktas/Documents/GitHub/real_estate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813748D4-16BD-E748-9696-83C55CF53BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EB62DF-34EA-9440-875F-E119C8B6D61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="1020" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Subject</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>Completed location, search, house feed, ordering houses, animations for detail screen and localization. House fetching  and business logic unit tests</t>
+  </si>
+  <si>
+    <t>User story 3 completed</t>
+  </si>
+  <si>
+    <t>Everything explained on story 3 implemented such as map, house detail, and url launchers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User story 4 completed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Made design, and link </t>
   </si>
 </sst>
 </file>
@@ -1726,7 +1738,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1823,19 +1835,35 @@
       <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="15"/>
+    <row r="7" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="17">
+        <v>5</v>
+      </c>
+      <c r="C7" s="18">
+        <v>45494</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>15</v>
+      </c>
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="15"/>
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="17">
+        <v>3</v>
+      </c>
+      <c r="C8" s="18">
+        <v>45494</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
@@ -2013,7 +2041,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>16.5</v>
+        <v>24.5</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
add dark mode working hours
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
+++ b/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umutaktas/Documents/GitHub/real_estate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EB62DF-34EA-9440-875F-E119C8B6D61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF1929D-CA92-5442-8496-F46525AD5623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Subject</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t xml:space="preserve">Made design, and link </t>
+  </si>
+  <si>
+    <t>Dark theme completed</t>
+  </si>
+  <si>
+    <t>Implemented dark theme through all app.</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1744,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1868,10 +1874,18 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="17">
+        <v>3</v>
+      </c>
+      <c r="C9" s="18">
+        <v>45497</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
@@ -2041,7 +2055,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>24.5</v>
+        <v>27.5</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
add no internet working hours
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
+++ b/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umutaktas/Documents/GitHub/real_estate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF1929D-CA92-5442-8496-F46525AD5623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CE84F6-EDED-5345-AB9B-488CB2AA585D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Subject</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Implemented dark theme through all app.</t>
+  </si>
+  <si>
+    <t>No internet Implemented</t>
+  </si>
+  <si>
+    <t>When there is no internet app fetches houses from local storage, map shows warning.</t>
   </si>
 </sst>
 </file>
@@ -1743,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="214" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1889,11 +1895,19 @@
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="15"/>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="17">
+        <v>2</v>
+      </c>
+      <c r="C10" s="18">
+        <v>45500</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>21</v>
+      </c>
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
@@ -2055,7 +2069,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>27.5</v>
+        <v>29.5</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
add wish list hours
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
+++ b/DTT-Assessment-Hour-Log- Umut-Aktas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umutaktas/Documents/GitHub/real_estate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CE84F6-EDED-5345-AB9B-488CB2AA585D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5903D729-190A-1B49-889F-BB1BE12434C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Subject</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>When there is no internet app fetches houses from local storage, map shows warning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wish list feature developed </t>
+  </si>
+  <si>
+    <t>28.97.2024</t>
+  </si>
+  <si>
+    <t>Created a new page for wishlist, add like functionaility. Liked houses is saved to phone storage.</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1759,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="214" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1911,11 +1920,19 @@
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="15"/>
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="17">
+        <v>4</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
@@ -2069,7 +2086,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>29.5</v>
+        <v>33.5</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>